<commit_message>
log loss example updated
</commit_message>
<xml_diff>
--- a/ML_Unit2/excel/Numerical Examples.xlsx
+++ b/ML_Unit2/excel/Numerical Examples.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/consulting/dono/idma_pt_public/ML_Unit2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/consulting/dono/idma_pt_public/ML_Unit2/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1265" documentId="8_{B53E1358-04C0-F346-8623-2140053B0E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED41D542-930F-C042-A7D3-D9EFE80FC08F}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="14_{78CFF5E8-614B-D648-B9A4-814B6632179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{908C272E-B49C-D048-B25F-903C2BC20D17}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" firstSheet="4" activeTab="10" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" firstSheet="5" activeTab="11" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
   </bookViews>
   <sheets>
     <sheet name="One Feature" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,11 @@
     <sheet name="Cross Validation" sheetId="12" r:id="rId9"/>
     <sheet name="User Item Rating Matrix" sheetId="13" r:id="rId10"/>
     <sheet name="Collaborative Filtering 1" sheetId="14" r:id="rId11"/>
+    <sheet name="Softmax Function" sheetId="15" r:id="rId12"/>
+    <sheet name="Log Loss" sheetId="16" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="93">
   <si>
     <t>x</t>
   </si>
@@ -284,6 +286,48 @@
   </si>
   <si>
     <t>lambda</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>Softmax</t>
+  </si>
+  <si>
+    <t>Probs</t>
+  </si>
+  <si>
+    <t>Actual Labels</t>
+  </si>
+  <si>
+    <t>Paid (0)</t>
+  </si>
+  <si>
+    <t>Default(1)</t>
+  </si>
+  <si>
+    <t>Late(2)</t>
+  </si>
+  <si>
+    <t>Prob_Paid</t>
+  </si>
+  <si>
+    <t>Prob_Default</t>
+  </si>
+  <si>
+    <t>Prob_Late</t>
+  </si>
+  <si>
+    <t>loss= -log(pi)</t>
   </si>
 </sst>
 </file>
@@ -597,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -708,21 +752,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -747,11 +776,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -761,11 +812,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9183,8 +9229,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>161719</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -9568,7 +9614,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -9657,8 +9703,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>101395</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -9784,7 +9830,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7">
@@ -10837,8 +10883,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>194733</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="TextBox 19">
@@ -10918,7 +10964,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="20" name="TextBox 19">
@@ -11320,6 +11366,1612 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>63148</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>23460</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="192616" cy="344453"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{933A7D9E-BD70-434E-AED9-9CACD346B5B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="63148" y="23460"/>
+              <a:ext cx="192616" cy="344453"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝚯</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝟎</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5" name="TextBox 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{933A7D9E-BD70-434E-AED9-9CACD346B5B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="63148" y="23460"/>
+              <a:ext cx="192616" cy="344453"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝚯_𝟎</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>771173</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>26458</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="463549" cy="353307"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C0BCDF-369D-DE4E-838B-6F10C75CD49E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="771173" y="26458"/>
+              <a:ext cx="463549" cy="353307"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝚯</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝟏</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C0BCDF-369D-DE4E-838B-6F10C75CD49E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="771173" y="26458"/>
+              <a:ext cx="463549" cy="353307"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝚯_𝟏</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>756004</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28927</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="463549" cy="353307"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC7A0DFD-17C7-5F4C-B55A-532FEAA8D914}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1585032" y="28927"/>
+              <a:ext cx="463549" cy="353307"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝚯</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝟐</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC7A0DFD-17C7-5F4C-B55A-532FEAA8D914}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1585032" y="28927"/>
+              <a:ext cx="463549" cy="353307"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝚯_𝟐</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+            </a:p>
+            <a:p>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>239536</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>146932</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2097818" cy="488082"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEFA2C7E-B2A4-124E-B707-3B46DF80BF6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2726619" y="2175404"/>
+              <a:ext cx="2097818" cy="488082"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑠𝑜𝑓𝑡𝑚𝑎𝑥</m:t>
+                    </m:r>
+                    <m:d>
+                      <m:dPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑋</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:e>
+                    </m:d>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:nary>
+                          <m:naryPr>
+                            <m:chr m:val="∑"/>
+                            <m:supHide m:val="on"/>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:naryPr>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                          <m:sup/>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t> </m:t>
+                            </m:r>
+                          </m:e>
+                        </m:nary>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>(</m:t>
+                        </m:r>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑒</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝜃</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑗</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>.</m:t>
+                            </m:r>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑋</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑖</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:sup>
+                        </m:sSup>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>)</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:m>
+                      <m:mPr>
+                        <m:mcs>
+                          <m:mc>
+                            <m:mcPr>
+                              <m:count m:val="1"/>
+                              <m:mcJc m:val="center"/>
+                            </m:mcPr>
+                          </m:mc>
+                        </m:mcs>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:mPr>
+                      <m:mr>
+                        <m:e>
+                          <m:sSup>
+                            <m:sSupPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:sSupPr>
+                            <m:e>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>𝑒</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:sup>
+                              <m:sSub>
+                                <m:sSubPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:sSubPr>
+                                <m:e>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:brk m:alnAt="7"/>
+                                    </m:rPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝜃</m:t>
+                                  </m:r>
+                                </m:e>
+                                <m:sub>
+                                  <m:r>
+                                    <m:rPr>
+                                      <m:brk m:alnAt="7"/>
+                                    </m:rPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>0</m:t>
+                                  </m:r>
+                                </m:sub>
+                              </m:sSub>
+                              <m:r>
+                                <m:rPr>
+                                  <m:brk m:alnAt="7"/>
+                                </m:rPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>.</m:t>
+                              </m:r>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>𝑋𝑖</m:t>
+                              </m:r>
+                            </m:sup>
+                          </m:sSup>
+                        </m:e>
+                      </m:mr>
+                      <m:mr>
+                        <m:e>
+                          <m:sSup>
+                            <m:sSupPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:sSupPr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>𝑒</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:sup>
+                              <m:sSub>
+                                <m:sSubPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:sSubPr>
+                                <m:e>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝜃</m:t>
+                                  </m:r>
+                                </m:e>
+                                <m:sub>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>1</m:t>
+                                  </m:r>
+                                </m:sub>
+                              </m:sSub>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>.</m:t>
+                              </m:r>
+                              <m:sSub>
+                                <m:sSubPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:sSubPr>
+                                <m:e>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝑋</m:t>
+                                  </m:r>
+                                </m:e>
+                                <m:sub>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝑖</m:t>
+                                  </m:r>
+                                </m:sub>
+                              </m:sSub>
+                            </m:sup>
+                          </m:sSup>
+                        </m:e>
+                      </m:mr>
+                      <m:mr>
+                        <m:e>
+                          <m:sSup>
+                            <m:sSupPr>
+                              <m:ctrlPr>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                              </m:ctrlPr>
+                            </m:sSupPr>
+                            <m:e>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>𝑒</m:t>
+                              </m:r>
+                            </m:e>
+                            <m:sup>
+                              <m:sSub>
+                                <m:sSubPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:sSubPr>
+                                <m:e>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝜃</m:t>
+                                  </m:r>
+                                </m:e>
+                                <m:sub>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝑛</m:t>
+                                  </m:r>
+                                </m:sub>
+                              </m:sSub>
+                              <m:r>
+                                <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                </a:rPr>
+                                <m:t>.</m:t>
+                              </m:r>
+                              <m:sSub>
+                                <m:sSubPr>
+                                  <m:ctrlPr>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                  </m:ctrlPr>
+                                </m:sSubPr>
+                                <m:e>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝑋</m:t>
+                                  </m:r>
+                                </m:e>
+                                <m:sub>
+                                  <m:r>
+                                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                    </a:rPr>
+                                    <m:t>𝑖</m:t>
+                                  </m:r>
+                                </m:sub>
+                              </m:sSub>
+                            </m:sup>
+                          </m:sSup>
+                        </m:e>
+                      </m:mr>
+                    </m:m>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEFA2C7E-B2A4-124E-B707-3B46DF80BF6E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2726619" y="2175404"/>
+              <a:ext cx="2097818" cy="488082"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠𝑜𝑓𝑡𝑚𝑎𝑥(𝑋_𝑖 )=1/(∑8_𝑗▒ (𝑒^(𝜃_𝑗.𝑋_𝑖 ))) ■8(𝑒^(𝜃_0.𝑋𝑖)@𝑒^(𝜃_1.𝑋_𝑖 )@𝑒^(𝜃_𝑛.𝑋_𝑖 ) )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>160161</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>41098</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="362343" cy="180690"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACCCC54-E46C-4D4E-9294-887D485CC850}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8450439" y="1055334"/>
+              <a:ext cx="362343" cy="180690"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝒆</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜽</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝟎</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>.</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑿</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝒊</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="9" name="TextBox 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACCCC54-E46C-4D4E-9294-887D485CC850}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8450439" y="1055334"/>
+              <a:ext cx="362343" cy="180690"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝒆^(𝜽_𝟎.𝑿_𝒊 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>74436</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>44097</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="357598" cy="156268"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148928E8-7597-2840-9E82-5571573857D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9193742" y="1058333"/>
+              <a:ext cx="357598" cy="156268"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝒆</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜽</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝟏</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>.</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑿</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝒊</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="10" name="TextBox 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{148928E8-7597-2840-9E82-5571573857D8}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9193742" y="1058333"/>
+              <a:ext cx="357598" cy="156268"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝒆^(𝜽_𝟏.𝑿_𝒊 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>37747</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="357598" cy="156268"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58A8603A-C693-B74A-9842-9D903458CFAA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10034059" y="1051983"/>
+              <a:ext cx="357598" cy="156268"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝒆</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜽</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝟐</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>.</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑿</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="en-US" sz="1100" b="1" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝒊</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="11" name="TextBox 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58A8603A-C693-B74A-9842-9D903458CFAA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10034059" y="1051983"/>
+              <a:ext cx="357598" cy="156268"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="1" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝒆^(𝜽_𝟐.𝑿_𝒊 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -18322,25 +19974,25 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="47" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="49"/>
-      <c r="B3" s="50" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="45" t="s">
         <v>60</v>
       </c>
     </row>
@@ -18360,7 +20012,7 @@
       <c r="E4" s="5">
         <v>4</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="46" t="s">
         <v>62</v>
       </c>
       <c r="H4" s="5" t="s">
@@ -18395,7 +20047,7 @@
       <c r="H5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="I5" s="53">
+      <c r="I5" s="48">
         <f>CORREL(B$6:E$6,B5:E5)</f>
         <v>0.30151134457776363</v>
       </c>
@@ -18426,7 +20078,7 @@
       <c r="H6" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I6" s="53">
+      <c r="I6" s="48">
         <f t="shared" ref="I6:I8" si="0">CORREL(B$6:E$6,B6:E6)</f>
         <v>1</v>
       </c>
@@ -18457,7 +20109,7 @@
       <c r="H7" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I7" s="53">
+      <c r="I7" s="48">
         <f t="shared" si="0"/>
         <v>-0.70710678118654746</v>
       </c>
@@ -18488,7 +20140,7 @@
       <c r="H8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="53">
+      <c r="I8" s="48">
         <f t="shared" si="0"/>
         <v>-0.14002800840280097</v>
       </c>
@@ -18498,22 +20150,22 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H10" s="54" t="s">
+      <c r="H10" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="50">
         <f>(F5*I5+F6*I6)/SUM(I5:I6)</f>
         <v>4.5366750419289197</v>
       </c>
-      <c r="J10" s="56">
+      <c r="J10" s="51">
         <f>(F5*J5+F6*J6)/SUM(J5:J6)</f>
         <v>4.0290032174596364</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="H11" s="54"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="58"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18525,393 +20177,393 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BF763C-C298-5541-BB88-0C28F95F00D9}">
   <dimension ref="B4:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScale="150" workbookViewId="0">
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="59">
+      <c r="B4" s="54">
         <v>1</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="59" t="s">
+      <c r="D4" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="59">
+      <c r="F4" s="54">
         <v>3</v>
       </c>
-      <c r="I4" s="59">
+      <c r="I4" s="54">
         <v>1</v>
       </c>
-      <c r="J4" s="59" t="s">
+      <c r="J4" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="K4" s="59" t="s">
+      <c r="K4" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="59" t="s">
+      <c r="L4" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="M4" s="59">
+      <c r="M4" s="54">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="59">
+      <c r="C5" s="54">
         <v>3</v>
       </c>
-      <c r="D5" s="59">
+      <c r="D5" s="54">
         <v>5</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="59">
+      <c r="F5" s="54">
         <v>1</v>
       </c>
-      <c r="I5" s="59" t="s">
+      <c r="I5" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J5" s="59">
+      <c r="J5" s="54">
         <v>3</v>
       </c>
-      <c r="K5" s="59">
+      <c r="K5" s="54">
         <v>5</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="59">
+      <c r="M5" s="54">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B6" s="59">
+      <c r="B6" s="54">
         <v>6</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="54">
         <v>6</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="54">
         <v>7</v>
       </c>
-      <c r="F6" s="59" t="s">
+      <c r="F6" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="I6" s="59">
+      <c r="I6" s="54">
         <v>6</v>
       </c>
-      <c r="J6" s="59">
+      <c r="J6" s="54">
         <v>6</v>
       </c>
-      <c r="K6" s="59" t="s">
+      <c r="K6" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="59">
+      <c r="L6" s="54">
         <v>7</v>
       </c>
-      <c r="M6" s="59" t="s">
+      <c r="M6" s="54" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="59">
+      <c r="D7" s="54">
         <v>7</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="59">
+      <c r="F7" s="54">
         <v>6</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J7" s="59" t="s">
+      <c r="J7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="59">
+      <c r="K7" s="54">
         <v>7</v>
       </c>
-      <c r="L7" s="59" t="s">
+      <c r="L7" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="59">
+      <c r="M7" s="54">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="59">
+      <c r="B8" s="54">
         <v>3</v>
       </c>
-      <c r="C8" s="59">
+      <c r="C8" s="54">
         <v>1</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="54">
         <v>6</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="I8" s="59">
+      <c r="I8" s="54">
         <v>3</v>
       </c>
-      <c r="J8" s="59">
+      <c r="J8" s="54">
         <v>1</v>
       </c>
-      <c r="K8" s="59" t="s">
+      <c r="K8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L8" s="59">
+      <c r="L8" s="54">
         <v>6</v>
       </c>
-      <c r="M8" s="59" t="s">
+      <c r="M8" s="54" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="54">
         <v>7</v>
       </c>
-      <c r="F9" s="59">
+      <c r="F9" s="54">
         <v>3</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="59" t="s">
+      <c r="J9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="59" t="s">
+      <c r="K9" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L9" s="59">
+      <c r="L9" s="54">
         <v>7</v>
       </c>
-      <c r="M9" s="59">
+      <c r="M9" s="54">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="59">
+      <c r="B10" s="54">
         <v>4</v>
       </c>
-      <c r="C10" s="59">
+      <c r="C10" s="54">
         <v>5</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="59">
+      <c r="F10" s="54">
         <v>3</v>
       </c>
-      <c r="I10" s="59">
+      <c r="I10" s="54">
         <v>4</v>
       </c>
-      <c r="J10" s="59">
+      <c r="J10" s="54">
         <v>5</v>
       </c>
-      <c r="K10" s="59" t="s">
+      <c r="K10" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L10" s="59" t="s">
+      <c r="L10" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="M10" s="59">
+      <c r="M10" s="54">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="59" t="s">
+      <c r="B11" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="59">
+      <c r="D11" s="54">
         <v>6</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E11" s="54">
         <v>7</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="54">
         <v>3</v>
       </c>
-      <c r="I11" s="59" t="s">
+      <c r="I11" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J11" s="59" t="s">
+      <c r="J11" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K11" s="54">
         <v>6</v>
       </c>
-      <c r="L11" s="59">
+      <c r="L11" s="54">
         <v>7</v>
       </c>
-      <c r="M11" s="59">
+      <c r="M11" s="54">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="59">
+      <c r="B12" s="54">
         <v>1</v>
       </c>
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="59">
+      <c r="D12" s="54">
         <v>5</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="59">
+      <c r="F12" s="54">
         <v>3</v>
       </c>
-      <c r="I12" s="59">
+      <c r="I12" s="54">
         <v>1</v>
       </c>
-      <c r="J12" s="59" t="s">
+      <c r="J12" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="54">
         <v>5</v>
       </c>
-      <c r="L12" s="59" t="s">
+      <c r="L12" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="M12" s="59">
+      <c r="M12" s="54">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="54">
         <v>4</v>
       </c>
-      <c r="F13" s="59">
+      <c r="F13" s="54">
         <v>7</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="59" t="s">
+      <c r="J13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="K13" s="59" t="s">
+      <c r="K13" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L13" s="59">
+      <c r="L13" s="54">
         <v>4</v>
       </c>
-      <c r="M13" s="59">
+      <c r="M13" s="54">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="59">
+      <c r="B14" s="54">
         <v>7</v>
       </c>
-      <c r="C14" s="59">
+      <c r="C14" s="54">
         <v>8</v>
       </c>
-      <c r="D14" s="59">
+      <c r="D14" s="54">
         <v>3</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="59">
+      <c r="I14" s="54">
         <v>7</v>
       </c>
-      <c r="J14" s="59">
+      <c r="J14" s="54">
         <v>8</v>
       </c>
-      <c r="K14" s="59">
+      <c r="K14" s="54">
         <v>3</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="M14" s="59" t="s">
+      <c r="M14" s="54" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="59">
+      <c r="C15" s="54">
         <v>1</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="59">
+      <c r="E15" s="54">
         <v>3</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="J15" s="59">
+      <c r="J15" s="54">
         <v>1</v>
       </c>
-      <c r="K15" s="59" t="s">
+      <c r="K15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="L15" s="59">
+      <c r="L15" s="54">
         <v>3</v>
       </c>
-      <c r="M15" s="59" t="s">
+      <c r="M15" s="54" t="s">
         <v>62</v>
       </c>
     </row>
@@ -18919,308 +20571,308 @@
       <c r="P20" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="Q20" s="60">
+      <c r="Q20" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="M23" s="59">
+      <c r="B23" s="54"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="M23" s="54">
         <f>I4/(1+$Q20)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="N23" s="59">
+      <c r="N23" s="54">
         <v>0</v>
       </c>
-      <c r="O23" s="59">
+      <c r="O23" s="54">
         <v>0</v>
       </c>
-      <c r="P23" s="59">
+      <c r="P23" s="54">
         <v>0</v>
       </c>
-      <c r="Q23" s="59">
-        <f t="shared" ref="N23:Q23" si="0">M4/(1+$Q20)</f>
+      <c r="Q23" s="54">
+        <f t="shared" ref="Q23" si="0">M4/(1+$Q20)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59"/>
-      <c r="M24" s="59">
+      <c r="B24" s="54"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="M24" s="54">
         <v>0</v>
       </c>
-      <c r="N24" s="59">
+      <c r="N24" s="54">
         <f t="shared" ref="N24:N34" si="1">J5/(1+$Q21)</f>
         <v>3</v>
       </c>
-      <c r="O24" s="59">
-        <f t="shared" ref="O24:O34" si="2">K5/(1+$Q21)</f>
+      <c r="O24" s="54">
+        <f t="shared" ref="O24:O33" si="2">K5/(1+$Q21)</f>
         <v>5</v>
       </c>
-      <c r="P24" s="59">
+      <c r="P24" s="54">
         <v>0</v>
       </c>
-      <c r="Q24" s="59">
-        <f t="shared" ref="Q24:Q34" si="3">M5/(1+$Q21)</f>
+      <c r="Q24" s="54">
+        <f t="shared" ref="Q24:Q32" si="3">M5/(1+$Q21)</f>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="59"/>
-      <c r="C25" s="59"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
-      <c r="F25" s="59"/>
-      <c r="M25" s="59">
-        <f t="shared" ref="M24:M34" si="4">I6/(1+$Q22)</f>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="M25" s="54">
+        <f t="shared" ref="M25:M33" si="4">I6/(1+$Q22)</f>
         <v>6</v>
       </c>
-      <c r="N25" s="59">
+      <c r="N25" s="54">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="O25" s="59">
+      <c r="O25" s="54">
         <v>0</v>
       </c>
-      <c r="P25" s="59">
-        <f t="shared" ref="P24:P34" si="5">L6/(1+$Q22)</f>
+      <c r="P25" s="54">
+        <f t="shared" ref="P25:P34" si="5">L6/(1+$Q22)</f>
         <v>7</v>
       </c>
-      <c r="Q25" s="59">
+      <c r="Q25" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="59"/>
-      <c r="C26" s="59"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="M26" s="59">
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="M26" s="54">
         <v>0</v>
       </c>
-      <c r="N26" s="59">
+      <c r="N26" s="54">
         <v>0</v>
       </c>
-      <c r="O26" s="59">
+      <c r="O26" s="54">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
-      <c r="P26" s="59">
+      <c r="P26" s="54">
         <v>0</v>
       </c>
-      <c r="Q26" s="59">
+      <c r="Q26" s="54">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="59"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="M27" s="59">
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="M27" s="54">
         <f t="shared" si="4"/>
         <v>1.5</v>
       </c>
-      <c r="N27" s="59">
+      <c r="N27" s="54">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="O27" s="59">
+      <c r="O27" s="54">
         <v>0</v>
       </c>
-      <c r="P27" s="59">
+      <c r="P27" s="54">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="Q27" s="59">
+      <c r="Q27" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
       <c r="G28" t="s">
         <v>76</v>
       </c>
       <c r="H28" t="s">
         <v>77</v>
       </c>
-      <c r="M28" s="59">
+      <c r="M28" s="54">
         <v>0</v>
       </c>
-      <c r="N28" s="59">
+      <c r="N28" s="54">
         <v>0</v>
       </c>
-      <c r="O28" s="59">
+      <c r="O28" s="54">
         <v>0</v>
       </c>
-      <c r="P28" s="59">
+      <c r="P28" s="54">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="Q28" s="59">
+      <c r="Q28" s="54">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="M29" s="59">
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="M29" s="54">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N29" s="59">
+      <c r="N29" s="54">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
-      <c r="O29" s="59">
+      <c r="O29" s="54">
         <v>0</v>
       </c>
-      <c r="P29" s="59">
+      <c r="P29" s="54">
         <v>0</v>
       </c>
-      <c r="Q29" s="59">
+      <c r="Q29" s="54">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="M30" s="59">
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="54"/>
+      <c r="M30" s="54">
         <v>0</v>
       </c>
-      <c r="N30" s="59">
+      <c r="N30" s="54">
         <v>0</v>
       </c>
-      <c r="O30" s="59">
+      <c r="O30" s="54">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="P30" s="59">
+      <c r="P30" s="54">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="Q30" s="59">
+      <c r="Q30" s="54">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="M31" s="59">
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="M31" s="54">
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="N31" s="59">
+      <c r="N31" s="54">
         <v>0</v>
       </c>
-      <c r="O31" s="59">
+      <c r="O31" s="54">
         <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
-      <c r="P31" s="59">
+      <c r="P31" s="54">
         <v>0</v>
       </c>
-      <c r="Q31" s="59">
+      <c r="Q31" s="54">
         <f t="shared" si="3"/>
         <v>0.75</v>
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="M32" s="59">
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="M32" s="54">
         <v>0</v>
       </c>
-      <c r="N32" s="59">
+      <c r="N32" s="54">
         <v>0</v>
       </c>
-      <c r="O32" s="59">
+      <c r="O32" s="54">
         <v>0</v>
       </c>
-      <c r="P32" s="59">
+      <c r="P32" s="54">
         <f t="shared" si="5"/>
         <v>2.2857142857142856</v>
       </c>
-      <c r="Q32" s="59">
+      <c r="Q32" s="54">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="M33" s="59">
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="M33" s="54">
         <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
-      <c r="N33" s="59">
+      <c r="N33" s="54">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O33" s="59">
+      <c r="O33" s="54">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-      <c r="P33" s="59">
+      <c r="P33" s="54">
         <v>0</v>
       </c>
-      <c r="Q33" s="59">
+      <c r="Q33" s="54">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B34" s="59"/>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="M34" s="59">
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="M34" s="54">
         <v>0</v>
       </c>
-      <c r="N34" s="59">
+      <c r="N34" s="54">
         <f t="shared" si="1"/>
         <v>0.5714285714285714</v>
       </c>
-      <c r="O34" s="59">
+      <c r="O34" s="54">
         <v>0</v>
       </c>
-      <c r="P34" s="59">
+      <c r="P34" s="54">
         <f t="shared" si="5"/>
         <v>1.7142857142857142</v>
       </c>
-      <c r="Q34" s="59">
+      <c r="Q34" s="54">
         <v>0</v>
       </c>
     </row>
@@ -19233,6 +20885,297 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2989B655-2B22-DF49-915B-BB07AA5416D8}">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="36">
+        <v>1E-3</v>
+      </c>
+      <c r="B2" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="36">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="36">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="B3" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="36">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="36">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="B4" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="36">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
+        <v>5.0000000000000003E-10</v>
+      </c>
+      <c r="B5" s="36">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="36">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E6" s="56" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="G6" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
+      <c r="M6" s="55"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D7" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="36">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="36">
+        <v>1</v>
+      </c>
+      <c r="G7" s="36">
+        <v>4</v>
+      </c>
+      <c r="H7" s="36">
+        <v>7</v>
+      </c>
+      <c r="I7" s="36">
+        <v>0</v>
+      </c>
+      <c r="K7" s="55">
+        <f>EXP(A2*E7+A3*F7+A4*G7+A5*H7)</f>
+        <v>1.0002400323031442</v>
+      </c>
+      <c r="L7" s="55">
+        <f>EXP(B2*E7+B3*F7+B4*G7+B5*H7)</f>
+        <v>67.356539810116573</v>
+      </c>
+      <c r="M7" s="55">
+        <f>EXP(C2*E7+C3*F7+C4*G7+C5+H7)</f>
+        <v>1314.2218231769091</v>
+      </c>
+      <c r="N7" s="47">
+        <f>SUM(K7:M7)</f>
+        <v>1382.5786030193287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D8" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="36">
+        <v>2</v>
+      </c>
+      <c r="G8" s="36">
+        <v>5</v>
+      </c>
+      <c r="H8" s="36">
+        <v>8</v>
+      </c>
+      <c r="I8" s="36">
+        <v>1</v>
+      </c>
+      <c r="O8" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="P8" s="56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="D9" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="36">
+        <v>0.3</v>
+      </c>
+      <c r="F9" s="36">
+        <v>3</v>
+      </c>
+      <c r="G9" s="36">
+        <v>6</v>
+      </c>
+      <c r="H9" s="36">
+        <v>9</v>
+      </c>
+      <c r="I9" s="36">
+        <v>2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" s="55">
+        <f>K7/N7</f>
+        <v>7.2345979470446106E-4</v>
+      </c>
+      <c r="P9" s="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O10" s="55">
+        <f>L7/N7</f>
+        <v>4.8718054556189973E-2</v>
+      </c>
+      <c r="P10" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O11" s="55">
+        <f>M7/N7</f>
+        <v>0.95055848564910561</v>
+      </c>
+      <c r="P11" s="36">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F373D4-DC66-DA4B-B986-4288610D8640}">
+  <dimension ref="B3:G6"/>
+  <sheetViews>
+    <sheetView zoomScale="166" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="G4" s="55">
+        <f>-LOG(D4)</f>
+        <v>0.3979400086720376</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="E5" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="G5" s="55">
+        <f>-LOG(E5)</f>
+        <v>0.69897000433601875</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="E6" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="55">
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="55">
+        <f>-LOG(F6)</f>
+        <v>0.3979400086720376</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -24724,7 +26667,7 @@
       <c r="B4" s="37">
         <v>-10.823492</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="62" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="42"/>
@@ -24754,7 +26697,7 @@
       <c r="B5" s="37">
         <v>-14.141714</v>
       </c>
-      <c r="C5" s="48"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="42"/>
       <c r="E5" s="38">
         <v>-0.24069299999999999</v>
@@ -24782,7 +26725,7 @@
       <c r="B6" s="37">
         <v>-32.409433999999997</v>
       </c>
-      <c r="C6" s="48"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="42"/>
       <c r="E6" s="38">
         <v>-0.48590919999999999</v>
@@ -24810,7 +26753,7 @@
       <c r="B7" s="37">
         <v>-9.0656832999999999</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="42"/>
       <c r="E7" s="38">
         <v>-0.1076836</v>
@@ -24838,7 +26781,7 @@
       <c r="B8" s="37">
         <v>-116.62475999999999</v>
       </c>
-      <c r="C8" s="48"/>
+      <c r="C8" s="62"/>
       <c r="D8" s="42"/>
       <c r="E8" s="38">
         <v>-1.6807323999999999</v>
@@ -24872,7 +26815,7 @@
       <c r="F9" s="37">
         <v>-78.386308999999997</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="62" t="s">
         <v>52</v>
       </c>
       <c r="H9" s="42"/>
@@ -24902,7 +26845,7 @@
       <c r="F10" s="37">
         <v>39.086097000000002</v>
       </c>
-      <c r="G10" s="48"/>
+      <c r="G10" s="62"/>
       <c r="H10" s="42"/>
       <c r="I10" s="38">
         <v>0.57477922999999997</v>
@@ -24930,7 +26873,7 @@
       <c r="F11" s="37">
         <v>-41.595868000000003</v>
       </c>
-      <c r="G11" s="48"/>
+      <c r="G11" s="62"/>
       <c r="H11" s="42"/>
       <c r="I11" s="38">
         <v>-0.55071340000000002</v>
@@ -24958,7 +26901,7 @@
       <c r="F12" s="37">
         <v>23.983129999999999</v>
       </c>
-      <c r="G12" s="48"/>
+      <c r="G12" s="62"/>
       <c r="H12" s="42"/>
       <c r="I12" s="38">
         <v>0.40179025000000002</v>
@@ -24986,7 +26929,7 @@
       <c r="F13" s="37">
         <v>-33.641916999999999</v>
       </c>
-      <c r="G13" s="48"/>
+      <c r="G13" s="62"/>
       <c r="H13" s="42"/>
       <c r="I13" s="38">
         <v>-0.50024550000000001</v>
@@ -25020,7 +26963,7 @@
       <c r="J14" s="39">
         <v>43.808776299999998</v>
       </c>
-      <c r="K14" s="44" t="s">
+      <c r="K14" s="58" t="s">
         <v>53</v>
       </c>
       <c r="L14" s="43"/>
@@ -25050,7 +26993,7 @@
       <c r="J15" s="39">
         <v>131.71287699999999</v>
       </c>
-      <c r="K15" s="45"/>
+      <c r="K15" s="59"/>
       <c r="L15" s="43"/>
       <c r="M15" s="40">
         <v>1.8261192500000001</v>
@@ -25078,7 +27021,7 @@
       <c r="J16" s="39">
         <v>16.181805300000001</v>
       </c>
-      <c r="K16" s="45"/>
+      <c r="K16" s="59"/>
       <c r="L16" s="43"/>
       <c r="M16" s="40">
         <v>0.30039895</v>
@@ -25106,7 +27049,7 @@
       <c r="J17" s="39">
         <v>-72.612886000000003</v>
       </c>
-      <c r="K17" s="45"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="43"/>
       <c r="M17" s="40">
         <v>-1.0550704</v>
@@ -25134,7 +27077,7 @@
       <c r="J18" s="39">
         <v>-91.941316999999998</v>
       </c>
-      <c r="K18" s="46"/>
+      <c r="K18" s="60"/>
       <c r="L18" s="43"/>
       <c r="M18" s="40">
         <v>-1.3722749000000001</v>
@@ -25168,7 +27111,7 @@
       <c r="N19" s="37">
         <v>-4.3803729999999996</v>
       </c>
-      <c r="O19" s="47" t="s">
+      <c r="O19" s="61" t="s">
         <v>54</v>
       </c>
     </row>
@@ -25197,7 +27140,7 @@
       <c r="N20" s="37">
         <v>97.5186128</v>
       </c>
-      <c r="O20" s="47"/>
+      <c r="O20" s="61"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -25224,7 +27167,7 @@
       <c r="N21" s="37">
         <v>-73.404396000000006</v>
       </c>
-      <c r="O21" s="47"/>
+      <c r="O21" s="61"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -25251,7 +27194,7 @@
       <c r="N22" s="37">
         <v>-81.747405000000001</v>
       </c>
-      <c r="O22" s="47"/>
+      <c r="O22" s="61"/>
       <c r="Q22" t="s">
         <v>55</v>
       </c>
@@ -25281,7 +27224,7 @@
       <c r="N23" s="37">
         <v>8.1673715199999997</v>
       </c>
-      <c r="O23" s="47"/>
+      <c r="O23" s="61"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -25316,7 +27259,7 @@
       <c r="B30" s="37">
         <v>-10.823492</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="62" t="s">
         <v>51</v>
       </c>
       <c r="D30" s="42"/>
@@ -25346,7 +27289,7 @@
       <c r="B31" s="37">
         <v>-14.141714</v>
       </c>
-      <c r="C31" s="48"/>
+      <c r="C31" s="62"/>
       <c r="D31" s="42"/>
       <c r="E31" s="38">
         <v>-0.24069299999999999</v>
@@ -25374,7 +27317,7 @@
       <c r="B32" s="37">
         <v>-32.409433999999997</v>
       </c>
-      <c r="C32" s="48"/>
+      <c r="C32" s="62"/>
       <c r="D32" s="42"/>
       <c r="E32" s="38">
         <v>-0.48590919999999999</v>
@@ -25402,7 +27345,7 @@
       <c r="B33" s="37">
         <v>-9.0656832999999999</v>
       </c>
-      <c r="C33" s="48"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="42"/>
       <c r="E33" s="38">
         <v>-0.1076836</v>
@@ -25430,7 +27373,7 @@
       <c r="B34" s="37">
         <v>-116.62475999999999</v>
       </c>
-      <c r="C34" s="48"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="42"/>
       <c r="E34" s="38">
         <v>-1.6807323999999999</v>
@@ -25464,7 +27407,7 @@
       <c r="F35" s="37">
         <v>-78.386308999999997</v>
       </c>
-      <c r="G35" s="48" t="s">
+      <c r="G35" s="62" t="s">
         <v>52</v>
       </c>
       <c r="H35" s="42"/>
@@ -25494,7 +27437,7 @@
       <c r="F36" s="37">
         <v>39.086097000000002</v>
       </c>
-      <c r="G36" s="48"/>
+      <c r="G36" s="62"/>
       <c r="H36" s="42"/>
       <c r="I36" s="38">
         <v>0.57477922999999997</v>
@@ -25522,7 +27465,7 @@
       <c r="F37" s="37">
         <v>-41.595868000000003</v>
       </c>
-      <c r="G37" s="48"/>
+      <c r="G37" s="62"/>
       <c r="H37" s="42"/>
       <c r="I37" s="38">
         <v>-0.55071340000000002</v>
@@ -25550,7 +27493,7 @@
       <c r="F38" s="37">
         <v>23.983129999999999</v>
       </c>
-      <c r="G38" s="48"/>
+      <c r="G38" s="62"/>
       <c r="H38" s="42"/>
       <c r="I38" s="38">
         <v>0.40179025000000002</v>
@@ -25578,7 +27521,7 @@
       <c r="F39" s="37">
         <v>-33.641916999999999</v>
       </c>
-      <c r="G39" s="48"/>
+      <c r="G39" s="62"/>
       <c r="H39" s="42"/>
       <c r="I39" s="38">
         <v>-0.50024550000000001</v>
@@ -25612,7 +27555,7 @@
       <c r="J40" s="39">
         <v>43.808776299999998</v>
       </c>
-      <c r="K40" s="44" t="s">
+      <c r="K40" s="58" t="s">
         <v>53</v>
       </c>
       <c r="L40" s="43"/>
@@ -25642,7 +27585,7 @@
       <c r="J41" s="39">
         <v>131.71287699999999</v>
       </c>
-      <c r="K41" s="45"/>
+      <c r="K41" s="59"/>
       <c r="L41" s="43"/>
       <c r="M41" s="40">
         <v>1.8261192500000001</v>
@@ -25670,7 +27613,7 @@
       <c r="J42" s="39">
         <v>16.181805300000001</v>
       </c>
-      <c r="K42" s="45"/>
+      <c r="K42" s="59"/>
       <c r="L42" s="43"/>
       <c r="M42" s="40">
         <v>0.30039895</v>
@@ -25698,7 +27641,7 @@
       <c r="J43" s="39">
         <v>-72.612886000000003</v>
       </c>
-      <c r="K43" s="45"/>
+      <c r="K43" s="59"/>
       <c r="L43" s="43"/>
       <c r="M43" s="40">
         <v>-1.0550704</v>
@@ -25726,7 +27669,7 @@
       <c r="J44" s="39">
         <v>-91.941316999999998</v>
       </c>
-      <c r="K44" s="46"/>
+      <c r="K44" s="60"/>
       <c r="L44" s="43"/>
       <c r="M44" s="40">
         <v>-1.3722749000000001</v>
@@ -25760,7 +27703,7 @@
       <c r="N45" s="37">
         <v>-4.3803729999999996</v>
       </c>
-      <c r="O45" s="47" t="s">
+      <c r="O45" s="61" t="s">
         <v>54</v>
       </c>
     </row>
@@ -25789,7 +27732,7 @@
       <c r="N46" s="37">
         <v>97.5186128</v>
       </c>
-      <c r="O46" s="47"/>
+      <c r="O46" s="61"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -25816,7 +27759,7 @@
       <c r="N47" s="37">
         <v>-73.404396000000006</v>
       </c>
-      <c r="O47" s="47"/>
+      <c r="O47" s="61"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -25843,7 +27786,7 @@
       <c r="N48" s="37">
         <v>-81.747405000000001</v>
       </c>
-      <c r="O48" s="47"/>
+      <c r="O48" s="61"/>
       <c r="Q48" t="s">
         <v>55</v>
       </c>
@@ -25873,7 +27816,7 @@
       <c r="N49" s="37">
         <v>8.1673715199999997</v>
       </c>
-      <c r="O49" s="47"/>
+      <c r="O49" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
16-10-21 class codes updated'
</commit_message>
<xml_diff>
--- a/ML_Unit2/excel/Numerical Examples.xlsx
+++ b/ML_Unit2/excel/Numerical Examples.xlsx
@@ -20930,8 +20930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2989B655-2B22-DF49-915B-BB07AA5416D8}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="D2" zoomScale="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
revision session codes updated
</commit_message>
<xml_diff>
--- a/ML_Unit2/excel/Numerical Examples.xlsx
+++ b/ML_Unit2/excel/Numerical Examples.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="109" documentId="14_{78CFF5E8-614B-D648-B9A4-814B6632179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9AA9B3F-99B0-C347-AE89-66C613863516}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" firstSheet="5" activeTab="12" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" activeTab="6" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
   </bookViews>
   <sheets>
     <sheet name="One Feature" sheetId="1" r:id="rId1"/>
@@ -21171,7 +21171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F373D4-DC66-DA4B-B986-4288610D8640}">
   <dimension ref="B3:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+    <sheetView zoomScale="166" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -25464,8 +25464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC746A95-0158-0F4D-B669-7A3265AEC378}">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added initial project demo files
</commit_message>
<xml_diff>
--- a/ML_Unit2/excel/Numerical Examples.xlsx
+++ b/ML_Unit2/excel/Numerical Examples.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="109" documentId="14_{78CFF5E8-614B-D648-B9A4-814B6632179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9AA9B3F-99B0-C347-AE89-66C613863516}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" activeTab="6" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" activeTab="5" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
   </bookViews>
   <sheets>
     <sheet name="One Feature" sheetId="1" r:id="rId1"/>
@@ -25037,7 +25037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E5049-30EC-4A40-AFBE-945907B1D82E}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView topLeftCell="F11" zoomScale="200" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="200" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -25464,7 +25464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC746A95-0158-0F4D-B669-7A3265AEC378}">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" workbookViewId="0">
+    <sheetView zoomScale="166" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
18_01_22 class codes pushed
</commit_message>
<xml_diff>
--- a/ML_Unit2/excel/Numerical Examples.xlsx
+++ b/ML_Unit2/excel/Numerical Examples.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="109" documentId="14_{78CFF5E8-614B-D648-B9A4-814B6632179A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9AA9B3F-99B0-C347-AE89-66C613863516}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" activeTab="5" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
+    <workbookView minimized="1" xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15520" xr2:uid="{ECAB7E24-608D-CE4D-8CF3-A67A0795359D}"/>
   </bookViews>
   <sheets>
     <sheet name="One Feature" sheetId="1" r:id="rId1"/>
@@ -19524,8 +19524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CAED4E-A516-C449-AC80-EC93879FD305}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
+      <selection sqref="A1:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25037,7 +25037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7E5049-30EC-4A40-AFBE-945907B1D82E}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="200" zoomScaleNormal="210" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="200" zoomScaleNormal="210" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>

</xml_diff>